<commit_message>
merging sidejobs, parliament_periods and candidate_mandates
</commit_message>
<xml_diff>
--- a/AW_scraper/files/parliaments.xlsx
+++ b/AW_scraper/files/parliaments.xlsx
@@ -542,7 +542,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Sachsen 2019 - 2024</t>
+          <t>Sachsen 2024 - 2029</t>
         </is>
       </c>
     </row>
@@ -580,7 +580,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Brandenburg Wahl 2024</t>
+          <t>Brandenburg 2024 - 2029</t>
         </is>
       </c>
     </row>
@@ -618,7 +618,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Thüringen 2019 - 2024</t>
+          <t>Thüringen 2024 - 2029</t>
         </is>
       </c>
     </row>

</xml_diff>